<commit_message>
Edits to readme and lightbox supply list.
</commit_message>
<xml_diff>
--- a/lightbox/BerryBox_SupplyList.xlsx
+++ b/lightbox/BerryBox_SupplyList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usdagcc-my.sharepoint.com/personal/jeffrey_neyhart_usda_gov/Documents/Documents/CranberryLab/EquipmentSupplies/Phenomics/BerryBox/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usdagcc-my.sharepoint.com/personal/jeffrey_neyhart_usda_gov/Documents/Documents/CranberryLab/Phenomics/BerryBox/lightbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="13_ncr:1_{F44720A7-C9C0-43D5-A0DA-AB8B0010F368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8247FA32-C9E7-44F0-91CD-018B3B522A7C}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{F44720A7-C9C0-43D5-A0DA-AB8B0010F368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61F08B8C-1CF9-4263-9E64-A4998080AE2D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="125">
   <si>
     <t>class</t>
   </si>
@@ -388,6 +388,27 @@
   </si>
   <si>
     <t>custom machining: 457 mm x 610 mm (4); 457 mm x 457 mm (1); does not include shipping</t>
+  </si>
+  <si>
+    <t>aluminum u-channel, 1.75" base, 0.75" leg</t>
+  </si>
+  <si>
+    <t>6ALY6</t>
+  </si>
+  <si>
+    <t>https://usdaadvantage.gsa.gov/advantage/ws/catalog/product_detail?gsin=11000081328188</t>
+  </si>
+  <si>
+    <t>Grainger</t>
+  </si>
+  <si>
+    <t>camera mount</t>
+  </si>
+  <si>
+    <t>https://www.grainger.com/product/GRAINGER-APPROVED-U-Channel-6063-6ALY6</t>
+  </si>
+  <si>
+    <t>any u-channel with at least 0.75" leg and 1" width would suffice</t>
   </si>
 </sst>
 </file>
@@ -397,7 +418,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,6 +440,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -442,7 +468,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -453,6 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -737,7 +764,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +772,7 @@
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -811,6 +838,9 @@
         <f>F2*G2</f>
         <v>122.58</v>
       </c>
+      <c r="J2" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -1085,8 +1115,35 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H13" s="2"/>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" t="s">
+        <v>122</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>24.69</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>24.69</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="J13" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H14" s="2"/>
@@ -1402,7 +1459,7 @@
       <c r="G33" s="5"/>
       <c r="H33" s="6">
         <f>SUM(H2:H32)</f>
-        <v>447.82000000000005</v>
+        <v>472.51000000000005</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>